<commit_message>
Correcting date for wokisme dataset
</commit_message>
<xml_diff>
--- a/wokisme_pressenationalefr.xlsx
+++ b/wokisme_pressenationalefr.xlsx
@@ -407,7 +407,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>octobre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -440,7 +440,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>mai 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>février 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>décembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>juin 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>mars 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>mai 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>mars 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>mars 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>juin 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>juin 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>septembre 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>avril 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -795,7 +795,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>mars 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>mai 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>juillet 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>octobre 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>octobre 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>juillet 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>septembre 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>janvier 2025</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>juillet 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>février 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>août 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>février 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>janvier 2025</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>mars 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>juillet 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>novembre 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>novembre 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>juillet 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>août 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>juillet 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>novembre 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>mars 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>janvier 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>janvier 2025</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>janvier 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>août 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>mai 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>janvier 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>janvier 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>février 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>mars 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>janvier 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>octobre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>janvier 2025</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>décembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>décembre 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>avril 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>juillet 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>juillet 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>novembre 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>octobre 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>octobre 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>janvier 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>novembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>janvier 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>janvier 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>janvier 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2325,7 +2325,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>septembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>octobre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>novembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>décembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>décembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>décembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>septembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>septembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2684,7 +2684,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>février 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>décembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>novembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>novembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>décembre 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>décembre 2024</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>mars 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>mars 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2959,7 +2959,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>juin 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>juin 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>septembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>septembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>décembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>novembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>novembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>juin 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3379,7 +3379,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3445,7 +3445,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>janvier 2022</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>novembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>octobre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>octobre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3590,7 +3590,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>avril 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>octobre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>décembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -3755,7 +3755,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3816,7 +3816,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>mai 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3882,7 +3882,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>juin 2023</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>octobre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>septembre 2021</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">

</xml_diff>